<commit_message>
Corregida numeración de elementos WBS
</commit_message>
<xml_diff>
--- a/Diccionario de la WBS.xlsx
+++ b/Diccionario de la WBS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7635" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="157">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -31,12 +31,6 @@
     <t xml:space="preserve">Entregables </t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.2 </t>
-  </si>
-  <si>
     <t>Calidad</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>Planificacion</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.3 </t>
-  </si>
-  <si>
     <t>Proceso para definir el curso de accion requerido para alcanzar los objetivos del proyecto</t>
   </si>
   <si>
@@ -112,12 +103,6 @@
     <t>Procesos para completar o cerrar formalmente el proyecto, la fase o el contrato.</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.5 </t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -199,9 +184,6 @@
     <t>1.2.2</t>
   </si>
   <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
     <t>1.3.1</t>
   </si>
   <si>
@@ -212,30 +194,6 @@
   </si>
   <si>
     <t>1.4.2</t>
-  </si>
-  <si>
-    <t>1.4.2.1</t>
-  </si>
-  <si>
-    <t>1.4.2.2</t>
-  </si>
-  <si>
-    <t>1.4.2.3</t>
-  </si>
-  <si>
-    <t>1.4.2.4</t>
-  </si>
-  <si>
-    <t>1.4.3</t>
-  </si>
-  <si>
-    <t>1.4.4</t>
-  </si>
-  <si>
-    <t>1.4.5</t>
-  </si>
-  <si>
-    <t>1.4.6</t>
   </si>
   <si>
     <t>1.5.1</t>
@@ -433,9 +391,6 @@
     <t>Interfaz de los ABMs</t>
   </si>
   <si>
-    <t>Vistas de los ABMs</t>
-  </si>
-  <si>
     <t>Interfaz del home principal</t>
   </si>
   <si>
@@ -497,6 +452,78 @@
   </si>
   <si>
     <t>Que se cumplan los tiempos de planificacion y prevenir errores,  perdidas revisando y evaluando cada etapa</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Categorias y subcategorías</t>
+  </si>
+  <si>
+    <t>Vistas para los ABMs</t>
+  </si>
+  <si>
+    <t>1.3.2.1</t>
+  </si>
+  <si>
+    <t>1.3.2.2</t>
+  </si>
+  <si>
+    <t>1.3.2.3</t>
+  </si>
+  <si>
+    <t>1.3.2.4</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
+  </si>
+  <si>
+    <t>1.3.5</t>
+  </si>
+  <si>
+    <t>1.3.6</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.6.3</t>
+  </si>
+  <si>
+    <t>1.6.4</t>
+  </si>
+  <si>
+    <t>1.6.5</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.7.5</t>
   </si>
 </sst>
 </file>
@@ -968,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +1012,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1005,33 +1032,33 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1039,692 +1066,707 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>1.1000000000000001</v>
+      <c r="A6" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" t="s">
-        <v>142</v>
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
+        <v>112</v>
+      </c>
     </row>
     <row r="10" spans="1:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
     <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1.2</v>
+    </row>
+    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
-        <v>81</v>
+      <c r="C12" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>80</v>
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.3</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>106</v>
+        <v>139</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>82</v>
+        <v>40</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>83</v>
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1.4</v>
+      <c r="A19" t="s">
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>85</v>
+        <v>43</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
+        <v>44</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>48</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>92</v>
+        <v>50</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>93</v>
+        <v>51</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
         <v>94</v>
       </c>
-      <c r="D29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1.5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="C32" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>102</v>
-      </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1.6</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
+      </c>
+      <c r="G38" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1.7</v>
-      </c>
-      <c r="B36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="12"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>117</v>
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G10:S10"/>
-    <mergeCell ref="G11:S11"/>
-    <mergeCell ref="G9:S9"/>
+    <mergeCell ref="G40:S40"/>
+    <mergeCell ref="G41:S41"/>
+    <mergeCell ref="G39:S39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>